<commit_message>
Added the CDD Abbrreviation
</commit_message>
<xml_diff>
--- a/ACS_Abbravation.xlsx
+++ b/ACS_Abbravation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Air-Conditioner-Screen-Team-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ismail samy\Desktop\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{41337ABA-8C6A-46A5-A28C-7DAE6678B6DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve"> Air Conditioner Screen Abbreviations</t>
   </si>
@@ -173,11 +174,17 @@
     <t>It is a hierarchical and incremental decomposition of the project into phases,
 deliverables and work packages</t>
   </si>
+  <si>
+    <t>CDD</t>
+  </si>
+  <si>
+    <t>Component Design Document</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -277,21 +284,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,230 +578,238 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="96.85546875" customWidth="1"/>
-    <col min="3" max="3" width="72.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="96.88671875" customWidth="1"/>
+    <col min="3" max="3" width="72.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>